<commit_message>
Baically done with manual analysis module, just doing excel output now.
</commit_message>
<xml_diff>
--- a/fantasy_league_stats.xlsx
+++ b/fantasy_league_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\PycharmProjects\oct25_fantasy_stats_with_scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6088394-F36F-433F-873B-9FC3B9AC0227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE027377-C9AC-416F-B169-55E36E8F86B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4848" yWindow="0" windowWidth="14412" windowHeight="13680" xr2:uid="{5D12E0C9-41C9-4FE4-9360-174E34DB173A}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{5D12E0C9-41C9-4FE4-9360-174E34DB173A}"/>
   </bookViews>
   <sheets>
     <sheet name="Fantasy League Stats" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="79">
   <si>
     <t>Year</t>
   </si>
@@ -1138,10 +1138,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7048027D-AA2C-408F-94F9-6ABEB4298CC0}">
   <dimension ref="A1:BQ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="BQ55" sqref="BQ55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10965,6 +10965,30 @@
       <c r="BI50">
         <v>85.86</v>
       </c>
+      <c r="BJ50" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK50">
+        <v>108.22</v>
+      </c>
+      <c r="BL50" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM50">
+        <v>74.239999999999995</v>
+      </c>
+      <c r="BN50" t="s">
+        <v>3</v>
+      </c>
+      <c r="BO50">
+        <v>110.56</v>
+      </c>
+      <c r="BP50" t="s">
+        <v>4</v>
+      </c>
+      <c r="BQ50">
+        <v>90.14</v>
+      </c>
     </row>
     <row r="51" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
@@ -11147,6 +11171,30 @@
       <c r="BI51">
         <v>134.97999999999999</v>
       </c>
+      <c r="BJ51" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK51">
+        <v>129.26</v>
+      </c>
+      <c r="BL51" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM51">
+        <v>129.38</v>
+      </c>
+      <c r="BN51" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO51">
+        <v>95.88</v>
+      </c>
+      <c r="BP51" t="s">
+        <v>2</v>
+      </c>
+      <c r="BQ51">
+        <v>146.74</v>
+      </c>
     </row>
     <row r="52" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
@@ -11329,6 +11377,30 @@
       <c r="BI52">
         <v>92.16</v>
       </c>
+      <c r="BJ52" t="s">
+        <v>10</v>
+      </c>
+      <c r="BK52">
+        <v>150.28</v>
+      </c>
+      <c r="BL52" t="s">
+        <v>8</v>
+      </c>
+      <c r="BM52">
+        <v>108.76</v>
+      </c>
+      <c r="BN52" t="s">
+        <v>10</v>
+      </c>
+      <c r="BO52">
+        <v>88.32</v>
+      </c>
+      <c r="BP52" t="s">
+        <v>1</v>
+      </c>
+      <c r="BQ52">
+        <v>125.72</v>
+      </c>
     </row>
     <row r="53" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
@@ -11511,6 +11583,30 @@
       <c r="BI53">
         <v>123.66</v>
       </c>
+      <c r="BJ53" t="s">
+        <v>5</v>
+      </c>
+      <c r="BK53">
+        <v>106.98</v>
+      </c>
+      <c r="BL53" t="s">
+        <v>1</v>
+      </c>
+      <c r="BM53">
+        <v>124.94</v>
+      </c>
+      <c r="BN53" t="s">
+        <v>8</v>
+      </c>
+      <c r="BO53">
+        <v>109.28</v>
+      </c>
+      <c r="BP53" t="s">
+        <v>5</v>
+      </c>
+      <c r="BQ53">
+        <v>156.88</v>
+      </c>
     </row>
     <row r="54" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
@@ -11692,6 +11788,18 @@
       </c>
       <c r="BI54">
         <v>124.1</v>
+      </c>
+      <c r="BN54" t="s">
+        <v>7</v>
+      </c>
+      <c r="BO54">
+        <v>92.72</v>
+      </c>
+      <c r="BP54" t="s">
+        <v>6</v>
+      </c>
+      <c r="BQ54">
+        <v>87.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Baically done with manual analysis module, just doing excel output now. Plus minor bug fixes
</commit_message>
<xml_diff>
--- a/fantasy_league_stats.xlsx
+++ b/fantasy_league_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\PycharmProjects\oct25_fantasy_stats_with_scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6088394-F36F-433F-873B-9FC3B9AC0227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE027377-C9AC-416F-B169-55E36E8F86B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4848" yWindow="0" windowWidth="14412" windowHeight="13680" xr2:uid="{5D12E0C9-41C9-4FE4-9360-174E34DB173A}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{5D12E0C9-41C9-4FE4-9360-174E34DB173A}"/>
   </bookViews>
   <sheets>
     <sheet name="Fantasy League Stats" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="79">
   <si>
     <t>Year</t>
   </si>
@@ -1138,10 +1138,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7048027D-AA2C-408F-94F9-6ABEB4298CC0}">
   <dimension ref="A1:BQ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="BQ55" sqref="BQ55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10965,6 +10965,30 @@
       <c r="BI50">
         <v>85.86</v>
       </c>
+      <c r="BJ50" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK50">
+        <v>108.22</v>
+      </c>
+      <c r="BL50" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM50">
+        <v>74.239999999999995</v>
+      </c>
+      <c r="BN50" t="s">
+        <v>3</v>
+      </c>
+      <c r="BO50">
+        <v>110.56</v>
+      </c>
+      <c r="BP50" t="s">
+        <v>4</v>
+      </c>
+      <c r="BQ50">
+        <v>90.14</v>
+      </c>
     </row>
     <row r="51" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
@@ -11147,6 +11171,30 @@
       <c r="BI51">
         <v>134.97999999999999</v>
       </c>
+      <c r="BJ51" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK51">
+        <v>129.26</v>
+      </c>
+      <c r="BL51" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM51">
+        <v>129.38</v>
+      </c>
+      <c r="BN51" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO51">
+        <v>95.88</v>
+      </c>
+      <c r="BP51" t="s">
+        <v>2</v>
+      </c>
+      <c r="BQ51">
+        <v>146.74</v>
+      </c>
     </row>
     <row r="52" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
@@ -11329,6 +11377,30 @@
       <c r="BI52">
         <v>92.16</v>
       </c>
+      <c r="BJ52" t="s">
+        <v>10</v>
+      </c>
+      <c r="BK52">
+        <v>150.28</v>
+      </c>
+      <c r="BL52" t="s">
+        <v>8</v>
+      </c>
+      <c r="BM52">
+        <v>108.76</v>
+      </c>
+      <c r="BN52" t="s">
+        <v>10</v>
+      </c>
+      <c r="BO52">
+        <v>88.32</v>
+      </c>
+      <c r="BP52" t="s">
+        <v>1</v>
+      </c>
+      <c r="BQ52">
+        <v>125.72</v>
+      </c>
     </row>
     <row r="53" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
@@ -11511,6 +11583,30 @@
       <c r="BI53">
         <v>123.66</v>
       </c>
+      <c r="BJ53" t="s">
+        <v>5</v>
+      </c>
+      <c r="BK53">
+        <v>106.98</v>
+      </c>
+      <c r="BL53" t="s">
+        <v>1</v>
+      </c>
+      <c r="BM53">
+        <v>124.94</v>
+      </c>
+      <c r="BN53" t="s">
+        <v>8</v>
+      </c>
+      <c r="BO53">
+        <v>109.28</v>
+      </c>
+      <c r="BP53" t="s">
+        <v>5</v>
+      </c>
+      <c r="BQ53">
+        <v>156.88</v>
+      </c>
     </row>
     <row r="54" spans="1:69" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
@@ -11692,6 +11788,18 @@
       </c>
       <c r="BI54">
         <v>124.1</v>
+      </c>
+      <c r="BN54" t="s">
+        <v>7</v>
+      </c>
+      <c r="BO54">
+        <v>92.72</v>
+      </c>
+      <c r="BP54" t="s">
+        <v>6</v>
+      </c>
+      <c r="BQ54">
+        <v>87.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>